<commit_message>
Update drug_db to v2
</commit_message>
<xml_diff>
--- a/dist/latest_version/drug_db.xlsx
+++ b/dist/latest_version/drug_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/368813f78804d80c/Desktop/Project-AtBS-Live/dist/latest_version/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_B5015F4DFF7835213F2D4C62DDAE01657979CFF2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E4BB8DB-A834-49F8-8BAA-834D99C19BAC}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_B5015F4DFF7835213F2D4C62DDAE01657979CFF2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4EC5D39-8C0B-44FE-A058-57347C6878B8}"/>
   <bookViews>
-    <workbookView xWindow="11130" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Drugs" sheetId="1" r:id="rId1"/>
@@ -2528,6 +2528,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2854,8 +2858,8 @@
   <dimension ref="A1:C430"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+      <pane ySplit="1" topLeftCell="A379" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G394" sqref="G394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7152,7 +7156,7 @@
         <v>639</v>
       </c>
       <c r="C390" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
@@ -7163,7 +7167,7 @@
         <v>637</v>
       </c>
       <c r="C391" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>